<commit_message>
It works! ... Kinda. There are some randomly highlighted matches that need looking into
</commit_message>
<xml_diff>
--- a/MatchColor/DataFiles/SampleMatches.xlsx
+++ b/MatchColor/DataFiles/SampleMatches.xlsx
@@ -356,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +418,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A14" si="0" xml:space="preserve"> A3+1</f>
+        <f t="shared" ref="A4:A27" si="0" xml:space="preserve"> A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
@@ -612,6 +612,240 @@
       </c>
       <c r="E14">
         <v>6209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>10862</v>
+      </c>
+      <c r="C15">
+        <v>11000</v>
+      </c>
+      <c r="D15">
+        <v>8424</v>
+      </c>
+      <c r="E15">
+        <v>4291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3708</v>
+      </c>
+      <c r="C16">
+        <v>9793</v>
+      </c>
+      <c r="D16">
+        <v>4753</v>
+      </c>
+      <c r="E16">
+        <v>6798</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6041</v>
+      </c>
+      <c r="C17">
+        <v>6504</v>
+      </c>
+      <c r="D17">
+        <v>10994</v>
+      </c>
+      <c r="E17">
+        <v>9278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>6816</v>
+      </c>
+      <c r="C18">
+        <v>5936</v>
+      </c>
+      <c r="D18">
+        <v>3781</v>
+      </c>
+      <c r="E18">
+        <v>8295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>4720</v>
+      </c>
+      <c r="C19">
+        <v>3147</v>
+      </c>
+      <c r="D19">
+        <v>8214</v>
+      </c>
+      <c r="E19">
+        <v>7785</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>4723</v>
+      </c>
+      <c r="C20">
+        <v>5815</v>
+      </c>
+      <c r="D20">
+        <v>4290</v>
+      </c>
+      <c r="E20">
+        <v>4781</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>8683</v>
+      </c>
+      <c r="C21">
+        <v>7161</v>
+      </c>
+      <c r="D21">
+        <v>8814</v>
+      </c>
+      <c r="E21">
+        <v>9272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>6901</v>
+      </c>
+      <c r="C22">
+        <v>4751</v>
+      </c>
+      <c r="D22">
+        <v>4546</v>
+      </c>
+      <c r="E22">
+        <v>5890</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>5681</v>
+      </c>
+      <c r="C23">
+        <v>9793</v>
+      </c>
+      <c r="D23">
+        <v>6209</v>
+      </c>
+      <c r="E23">
+        <v>6816</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>5936</v>
+      </c>
+      <c r="C24">
+        <v>10769</v>
+      </c>
+      <c r="D24">
+        <v>4720</v>
+      </c>
+      <c r="E24">
+        <v>6041</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4290</v>
+      </c>
+      <c r="C25">
+        <v>10862</v>
+      </c>
+      <c r="D25">
+        <v>4721</v>
+      </c>
+      <c r="E25">
+        <v>10994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>6798</v>
+      </c>
+      <c r="C26">
+        <v>7785</v>
+      </c>
+      <c r="D26">
+        <v>10997</v>
+      </c>
+      <c r="E26">
+        <v>8814</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>8295</v>
+      </c>
+      <c r="C27">
+        <v>4546</v>
+      </c>
+      <c r="D27">
+        <v>8214</v>
+      </c>
+      <c r="E27">
+        <v>7161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>